<commit_message>
Updated Results and CB calc
</commit_message>
<xml_diff>
--- a/Results/20250819__Cacao__AltaVerapaz/__Tmax__plus2C/20250819__Cacao__AltaVerapaz_adjusted_canopy_crop_composition_cb_metrics.xlsx
+++ b/Results/20250819__Cacao__AltaVerapaz/__Tmax__plus2C/20250819__Cacao__AltaVerapaz_adjusted_canopy_crop_composition_cb_metrics.xlsx
@@ -574,10 +574,10 @@
         <v>10413</v>
       </c>
       <c r="D2" s="2">
-        <v>991844.6800000001</v>
+        <v>991864.0699999999</v>
       </c>
       <c r="E2" s="2">
-        <v>645653.9</v>
+        <v>645673.29</v>
       </c>
       <c r="F2" s="2">
         <v>346190.78</v>
@@ -586,16 +586,16 @@
         <v>28880</v>
       </c>
       <c r="H2" s="2">
-        <v>28878.96</v>
+        <v>28880</v>
       </c>
       <c r="I2" s="2">
-        <v>28880.01</v>
+        <v>28880</v>
       </c>
       <c r="J2" s="2">
-        <v>28868.7</v>
+        <v>28880</v>
       </c>
       <c r="K2" s="2">
-        <v>981431.6800000001</v>
+        <v>981451.0699999999</v>
       </c>
       <c r="L2" s="2">
         <v>0</v>
@@ -630,37 +630,37 @@
         <v>5135</v>
       </c>
       <c r="D3" s="2">
-        <v>779679.17</v>
+        <v>812097.11</v>
       </c>
       <c r="E3" s="2">
-        <v>618944.17</v>
+        <v>651365.6800000001</v>
       </c>
       <c r="F3" s="2">
         <v>160731.44</v>
       </c>
       <c r="G3" s="2">
-        <v>22926.48</v>
+        <v>23651.42</v>
       </c>
       <c r="H3" s="2">
-        <v>22513.8</v>
+        <v>23641</v>
       </c>
       <c r="I3" s="2">
-        <v>22789.9</v>
+        <v>23652.02</v>
       </c>
       <c r="J3" s="2">
-        <v>21740.29</v>
+        <v>23556.64</v>
       </c>
       <c r="K3" s="2">
-        <v>774544.17</v>
+        <v>806962.11</v>
       </c>
       <c r="L3" s="2">
-        <v>-206887.52</v>
+        <v>-174488.96</v>
       </c>
       <c r="M3" s="1">
-        <v>-40.29</v>
+        <v>-33.98</v>
       </c>
       <c r="N3" s="2">
-        <v>-26709.73</v>
+        <v>5692.39</v>
       </c>
       <c r="O3" s="2">
         <v>-185459.35</v>
@@ -669,7 +669,7 @@
         <v>-5278</v>
       </c>
       <c r="Q3" s="2">
-        <v>-206891.08</v>
+        <v>-174488.96</v>
       </c>
       <c r="R3" s="1">
         <v>28.62</v>
@@ -686,37 +686,37 @@
         <v>7267</v>
       </c>
       <c r="D4" s="2">
-        <v>876462.53</v>
+        <v>893206.35</v>
       </c>
       <c r="E4" s="2">
-        <v>645668.55</v>
+        <v>662412.49</v>
       </c>
       <c r="F4" s="2">
         <v>230793.86</v>
       </c>
       <c r="G4" s="2">
-        <v>25574.08</v>
+        <v>26007.39</v>
       </c>
       <c r="H4" s="2">
-        <v>25474.48</v>
+        <v>26007.39</v>
       </c>
       <c r="I4" s="2">
-        <v>25570.9</v>
+        <v>26007.39</v>
       </c>
       <c r="J4" s="2">
-        <v>25076.07</v>
+        <v>26007.39</v>
       </c>
       <c r="K4" s="2">
-        <v>869195.53</v>
+        <v>885939.35</v>
       </c>
       <c r="L4" s="2">
-        <v>-112236.15</v>
+        <v>-95511.72</v>
       </c>
       <c r="M4" s="1">
-        <v>-15.44</v>
+        <v>-13.14</v>
       </c>
       <c r="N4" s="2">
-        <v>14.65</v>
+        <v>16739.2</v>
       </c>
       <c r="O4" s="2">
         <v>-115396.93</v>
@@ -725,7 +725,7 @@
         <v>-3146</v>
       </c>
       <c r="Q4" s="2">
-        <v>-112236.27</v>
+        <v>-95511.72</v>
       </c>
       <c r="R4" s="1">
         <v>45.97</v>
@@ -742,37 +742,37 @@
         <v>7748</v>
       </c>
       <c r="D5" s="2">
-        <v>915418.12</v>
+        <v>928237.5600000001</v>
       </c>
       <c r="E5" s="2">
-        <v>649593.02</v>
+        <v>662412.49</v>
       </c>
       <c r="F5" s="2">
         <v>265825.07</v>
       </c>
       <c r="G5" s="2">
-        <v>26684.46</v>
+        <v>27027.39</v>
       </c>
       <c r="H5" s="2">
-        <v>26628.75</v>
+        <v>27027.39</v>
       </c>
       <c r="I5" s="2">
-        <v>26686.52</v>
+        <v>27027.39</v>
       </c>
       <c r="J5" s="2">
-        <v>26354.04</v>
+        <v>27027.39</v>
       </c>
       <c r="K5" s="2">
-        <v>907670.12</v>
+        <v>920489.5600000001</v>
       </c>
       <c r="L5" s="2">
-        <v>-73761.56</v>
+        <v>-60961.51</v>
       </c>
       <c r="M5" s="1">
-        <v>-9.52</v>
+        <v>-7.87</v>
       </c>
       <c r="N5" s="2">
-        <v>3939.12</v>
+        <v>16739.2</v>
       </c>
       <c r="O5" s="2">
         <v>-80365.72</v>
@@ -781,7 +781,7 @@
         <v>-2665</v>
       </c>
       <c r="Q5" s="2">
-        <v>-73761.60000000001</v>
+        <v>-60961.51</v>
       </c>
       <c r="R5" s="1">
         <v>53.12</v>
@@ -798,37 +798,37 @@
         <v>8281</v>
       </c>
       <c r="D6" s="2">
-        <v>926490.78</v>
+        <v>938540.86</v>
       </c>
       <c r="E6" s="2">
-        <v>650362.41</v>
+        <v>662412.49</v>
       </c>
       <c r="F6" s="2">
         <v>276128.36</v>
       </c>
       <c r="G6" s="2">
-        <v>26994.69</v>
+        <v>27327.39</v>
       </c>
       <c r="H6" s="2">
-        <v>26961.33</v>
+        <v>27327.39</v>
       </c>
       <c r="I6" s="2">
-        <v>26995.89</v>
+        <v>27327.39</v>
       </c>
       <c r="J6" s="2">
-        <v>26777.1</v>
+        <v>27327.39</v>
       </c>
       <c r="K6" s="2">
-        <v>918209.78</v>
+        <v>930259.86</v>
       </c>
       <c r="L6" s="2">
-        <v>-63221.9</v>
+        <v>-51191.22</v>
       </c>
       <c r="M6" s="1">
-        <v>-7.63</v>
+        <v>-6.18</v>
       </c>
       <c r="N6" s="2">
-        <v>4708.51</v>
+        <v>16739.2</v>
       </c>
       <c r="O6" s="2">
         <v>-70062.42</v>
@@ -837,7 +837,7 @@
         <v>-2132</v>
       </c>
       <c r="Q6" s="2">
-        <v>-63221.91</v>
+        <v>-51191.22</v>
       </c>
       <c r="R6" s="1">
         <v>59.2</v>
@@ -854,37 +854,37 @@
         <v>8814</v>
       </c>
       <c r="D7" s="2">
-        <v>951599.96</v>
+        <v>961191.76</v>
       </c>
       <c r="E7" s="2">
-        <v>650743.6800000001</v>
+        <v>660335.48</v>
       </c>
       <c r="F7" s="2">
         <v>300856.28</v>
       </c>
       <c r="G7" s="2">
-        <v>27714.69</v>
+        <v>27986.92</v>
       </c>
       <c r="H7" s="2">
-        <v>27701.73</v>
+        <v>27986.92</v>
       </c>
       <c r="I7" s="2">
-        <v>27715.08</v>
+        <v>27986.92</v>
       </c>
       <c r="J7" s="2">
-        <v>27607.46</v>
+        <v>27986.92</v>
       </c>
       <c r="K7" s="2">
-        <v>942785.96</v>
+        <v>952377.76</v>
       </c>
       <c r="L7" s="2">
-        <v>-38645.72</v>
+        <v>-29073.31</v>
       </c>
       <c r="M7" s="1">
-        <v>-4.38</v>
+        <v>-3.3</v>
       </c>
       <c r="N7" s="2">
-        <v>5089.78</v>
+        <v>14662.2</v>
       </c>
       <c r="O7" s="2">
         <v>-45334.51</v>
@@ -893,7 +893,7 @@
         <v>-1599</v>
       </c>
       <c r="Q7" s="2">
-        <v>-38645.73</v>
+        <v>-29073.31</v>
       </c>
       <c r="R7" s="1">
         <v>67.70999999999999</v>
@@ -910,37 +910,37 @@
         <v>9347</v>
       </c>
       <c r="D8" s="2">
-        <v>962041.88</v>
+        <v>967492.05</v>
       </c>
       <c r="E8" s="2">
-        <v>650882.3100000001</v>
+        <v>656332.48</v>
       </c>
       <c r="F8" s="2">
         <v>311159.57</v>
       </c>
       <c r="G8" s="2">
-        <v>28014.69</v>
+        <v>28170.36</v>
       </c>
       <c r="H8" s="2">
-        <v>28009.14</v>
+        <v>28170.36</v>
       </c>
       <c r="I8" s="2">
-        <v>28014.79</v>
+        <v>28170.36</v>
       </c>
       <c r="J8" s="2">
-        <v>27956.84</v>
+        <v>28170.36</v>
       </c>
       <c r="K8" s="2">
-        <v>952694.88</v>
+        <v>958145.05</v>
       </c>
       <c r="L8" s="2">
-        <v>-28736.8</v>
+        <v>-23306.02</v>
       </c>
       <c r="M8" s="1">
-        <v>-3.07</v>
+        <v>-2.49</v>
       </c>
       <c r="N8" s="2">
-        <v>5228.41</v>
+        <v>10659.19</v>
       </c>
       <c r="O8" s="2">
         <v>-35031.21</v>
@@ -949,7 +949,7 @@
         <v>-1066</v>
       </c>
       <c r="Q8" s="2">
-        <v>-28736.8</v>
+        <v>-23306.02</v>
       </c>
       <c r="R8" s="1">
         <v>74.83</v>
@@ -966,37 +966,37 @@
         <v>9880</v>
       </c>
       <c r="D9" s="2">
-        <v>984966.05</v>
+        <v>988003.22</v>
       </c>
       <c r="E9" s="2">
-        <v>649078.5600000001</v>
+        <v>652115.73</v>
       </c>
       <c r="F9" s="2">
         <v>335887.49</v>
       </c>
       <c r="G9" s="2">
-        <v>28680.94</v>
+        <v>28767.58</v>
       </c>
       <c r="H9" s="2">
-        <v>28677.65</v>
+        <v>28767.58</v>
       </c>
       <c r="I9" s="2">
-        <v>28680.99</v>
+        <v>28767.58</v>
       </c>
       <c r="J9" s="2">
-        <v>28645.95</v>
+        <v>28767.58</v>
       </c>
       <c r="K9" s="2">
-        <v>975086.05</v>
+        <v>978123.22</v>
       </c>
       <c r="L9" s="2">
-        <v>-6345.63</v>
+        <v>-3327.85</v>
       </c>
       <c r="M9" s="1">
-        <v>-0.64</v>
+        <v>-0.34</v>
       </c>
       <c r="N9" s="2">
-        <v>3424.66</v>
+        <v>6442.44</v>
       </c>
       <c r="O9" s="2">
         <v>-10303.3</v>
@@ -1005,7 +1005,7 @@
         <v>-533</v>
       </c>
       <c r="Q9" s="2">
-        <v>-6345.63</v>
+        <v>-3327.85</v>
       </c>
       <c r="R9" s="1">
         <v>78.33</v>
@@ -1022,37 +1022,37 @@
         <v>10983</v>
       </c>
       <c r="D10" s="2">
-        <v>997422.39</v>
+        <v>994358.84</v>
       </c>
       <c r="E10" s="2">
-        <v>640928.3100000001</v>
+        <v>637864.76</v>
       </c>
       <c r="F10" s="2">
         <v>356494.08</v>
       </c>
       <c r="G10" s="2">
-        <v>29041.9</v>
+        <v>28952.64</v>
       </c>
       <c r="H10" s="2">
-        <v>29041.79</v>
+        <v>28952.64</v>
       </c>
       <c r="I10" s="2">
-        <v>29041.9</v>
+        <v>28952.64</v>
       </c>
       <c r="J10" s="2">
-        <v>29040.6</v>
+        <v>28952.64</v>
       </c>
       <c r="K10" s="2">
-        <v>986439.39</v>
+        <v>983375.84</v>
       </c>
       <c r="L10" s="2">
-        <v>5007.71</v>
+        <v>1924.77</v>
       </c>
       <c r="M10" s="1">
-        <v>0.46</v>
+        <v>0.18</v>
       </c>
       <c r="N10" s="2">
-        <v>-4725.59</v>
+        <v>-7808.53</v>
       </c>
       <c r="O10" s="2">
         <v>10303.3</v>
@@ -1061,7 +1061,7 @@
         <v>570</v>
       </c>
       <c r="Q10" s="2">
-        <v>5007.71</v>
+        <v>1924.77</v>
       </c>
       <c r="R10" s="1">
         <v>86.88</v>
@@ -1078,37 +1078,37 @@
         <v>11557</v>
       </c>
       <c r="D11" s="2">
-        <v>1017408.97</v>
+        <v>1011810.25</v>
       </c>
       <c r="E11" s="2">
-        <v>636186.97</v>
+        <v>630588.26</v>
       </c>
       <c r="F11" s="2">
         <v>381221.99</v>
       </c>
       <c r="G11" s="2">
-        <v>29623.79</v>
+        <v>29460.77</v>
       </c>
       <c r="H11" s="2">
-        <v>29623.79</v>
+        <v>29460.77</v>
       </c>
       <c r="I11" s="2">
-        <v>29623.79</v>
+        <v>29460.77</v>
       </c>
       <c r="J11" s="2">
-        <v>29623.79</v>
+        <v>29460.77</v>
       </c>
       <c r="K11" s="2">
-        <v>1005851.97</v>
+        <v>1000253.25</v>
       </c>
       <c r="L11" s="2">
-        <v>24420.29</v>
+        <v>18802.18</v>
       </c>
       <c r="M11" s="1">
-        <v>2.11</v>
+        <v>1.63</v>
       </c>
       <c r="N11" s="2">
-        <v>-9466.92</v>
+        <v>-15085.03</v>
       </c>
       <c r="O11" s="2">
         <v>35031.21</v>
@@ -1117,7 +1117,7 @@
         <v>1144</v>
       </c>
       <c r="Q11" s="2">
-        <v>24420.29</v>
+        <v>18802.18</v>
       </c>
       <c r="R11" s="1">
         <v>90.09999999999999</v>
@@ -1134,37 +1134,37 @@
         <v>12127</v>
       </c>
       <c r="D12" s="2">
-        <v>1020693.19</v>
+        <v>1011867.9</v>
       </c>
       <c r="E12" s="2">
-        <v>629167.9</v>
+        <v>620342.61</v>
       </c>
       <c r="F12" s="2">
         <v>391525.29</v>
       </c>
       <c r="G12" s="2">
-        <v>29719.41</v>
+        <v>29462.45</v>
       </c>
       <c r="H12" s="2">
-        <v>29719.41</v>
+        <v>29462.45</v>
       </c>
       <c r="I12" s="2">
-        <v>29719.41</v>
+        <v>29462.45</v>
       </c>
       <c r="J12" s="2">
-        <v>29719.41</v>
+        <v>29462.45</v>
       </c>
       <c r="K12" s="2">
-        <v>1008566.19</v>
+        <v>999740.9</v>
       </c>
       <c r="L12" s="2">
-        <v>27134.51</v>
+        <v>18289.83</v>
       </c>
       <c r="M12" s="1">
-        <v>2.24</v>
+        <v>1.51</v>
       </c>
       <c r="N12" s="2">
-        <v>-16486</v>
+        <v>-25330.68</v>
       </c>
       <c r="O12" s="2">
         <v>45334.51</v>
@@ -1173,7 +1173,7 @@
         <v>1714</v>
       </c>
       <c r="Q12" s="2">
-        <v>27134.51</v>
+        <v>18289.83</v>
       </c>
       <c r="R12" s="1">
         <v>91.53</v>
@@ -1190,37 +1190,37 @@
         <v>12701</v>
       </c>
       <c r="D13" s="2">
-        <v>1035345.29</v>
+        <v>1022544.64</v>
       </c>
       <c r="E13" s="2">
-        <v>619092.08</v>
+        <v>606291.4300000001</v>
       </c>
       <c r="F13" s="2">
         <v>416253.2</v>
       </c>
       <c r="G13" s="2">
-        <v>30146.04</v>
+        <v>29773.32</v>
       </c>
       <c r="H13" s="2">
-        <v>30146.04</v>
+        <v>29773.32</v>
       </c>
       <c r="I13" s="2">
-        <v>30146.04</v>
+        <v>29773.32</v>
       </c>
       <c r="J13" s="2">
-        <v>30146.04</v>
+        <v>29773.32</v>
       </c>
       <c r="K13" s="2">
-        <v>1022644.29</v>
+        <v>1009843.64</v>
       </c>
       <c r="L13" s="2">
-        <v>41212.6</v>
+        <v>28392.57</v>
       </c>
       <c r="M13" s="1">
-        <v>3.24</v>
+        <v>2.24</v>
       </c>
       <c r="N13" s="2">
-        <v>-26561.82</v>
+        <v>-39381.85</v>
       </c>
       <c r="O13" s="2">
         <v>70062.42</v>
@@ -1229,7 +1229,7 @@
         <v>2288</v>
       </c>
       <c r="Q13" s="2">
-        <v>41212.6</v>
+        <v>28392.57</v>
       </c>
       <c r="R13" s="1">
         <v>93.23</v>
@@ -1246,37 +1246,37 @@
         <v>13271</v>
       </c>
       <c r="D14" s="2">
-        <v>1037366.59</v>
+        <v>1021649.75</v>
       </c>
       <c r="E14" s="2">
-        <v>610810.09</v>
+        <v>595093.24</v>
       </c>
       <c r="F14" s="2">
         <v>426556.5</v>
       </c>
       <c r="G14" s="2">
-        <v>30204.89</v>
+        <v>29747.27</v>
       </c>
       <c r="H14" s="2">
-        <v>30204.89</v>
+        <v>29747.27</v>
       </c>
       <c r="I14" s="2">
-        <v>30204.89</v>
+        <v>29747.27</v>
       </c>
       <c r="J14" s="2">
-        <v>30204.89</v>
+        <v>29747.27</v>
       </c>
       <c r="K14" s="2">
-        <v>1024095.59</v>
+        <v>1008378.75</v>
       </c>
       <c r="L14" s="2">
-        <v>42663.91</v>
+        <v>26927.67</v>
       </c>
       <c r="M14" s="1">
-        <v>3.21</v>
+        <v>2.03</v>
       </c>
       <c r="N14" s="2">
-        <v>-34843.81</v>
+        <v>-50580.04</v>
       </c>
       <c r="O14" s="2">
         <v>80365.72</v>
@@ -1285,7 +1285,7 @@
         <v>2858</v>
       </c>
       <c r="Q14" s="2">
-        <v>42663.91</v>
+        <v>26927.67</v>
       </c>
       <c r="R14" s="1">
         <v>94.44</v>
@@ -1302,37 +1302,37 @@
         <v>13791</v>
       </c>
       <c r="D15" s="2">
-        <v>1059806.29</v>
+        <v>1040069.53</v>
       </c>
       <c r="E15" s="2">
-        <v>598218.5699999999</v>
+        <v>578481.8199999999</v>
       </c>
       <c r="F15" s="2">
         <v>461587.71</v>
       </c>
       <c r="G15" s="2">
-        <v>30858.27</v>
+        <v>30283.59</v>
       </c>
       <c r="H15" s="2">
-        <v>30858.27</v>
+        <v>30283.59</v>
       </c>
       <c r="I15" s="2">
-        <v>30858.27</v>
+        <v>30283.59</v>
       </c>
       <c r="J15" s="2">
-        <v>30858.27</v>
+        <v>30283.59</v>
       </c>
       <c r="K15" s="2">
-        <v>1046015.29</v>
+        <v>1026278.53</v>
       </c>
       <c r="L15" s="2">
-        <v>64583.6</v>
+        <v>44827.46</v>
       </c>
       <c r="M15" s="1">
-        <v>4.68</v>
+        <v>3.25</v>
       </c>
       <c r="N15" s="2">
-        <v>-47435.32</v>
+        <v>-67191.47</v>
       </c>
       <c r="O15" s="2">
         <v>115396.93</v>
@@ -1341,7 +1341,7 @@
         <v>3378</v>
       </c>
       <c r="Q15" s="2">
-        <v>64583.6</v>
+        <v>44827.46</v>
       </c>
       <c r="R15" s="1">
         <v>95.65000000000001</v>
@@ -1358,37 +1358,37 @@
         <v>16079</v>
       </c>
       <c r="D16" s="2">
-        <v>1079344.96</v>
+        <v>1046181.45</v>
       </c>
       <c r="E16" s="2">
-        <v>547694.8199999999</v>
+        <v>514531.32</v>
       </c>
       <c r="F16" s="2">
         <v>531650.13</v>
       </c>
       <c r="G16" s="2">
-        <v>31427.17</v>
+        <v>30461.55</v>
       </c>
       <c r="H16" s="2">
-        <v>31427.17</v>
+        <v>30461.55</v>
       </c>
       <c r="I16" s="2">
-        <v>31427.17</v>
+        <v>30461.55</v>
       </c>
       <c r="J16" s="2">
-        <v>31427.17</v>
+        <v>30461.55</v>
       </c>
       <c r="K16" s="2">
-        <v>1063265.96</v>
+        <v>1030102.45</v>
       </c>
       <c r="L16" s="2">
-        <v>81834.27</v>
+        <v>48651.38</v>
       </c>
       <c r="M16" s="1">
-        <v>5.09</v>
+        <v>3.03</v>
       </c>
       <c r="N16" s="2">
-        <v>-97959.07000000001</v>
+        <v>-131141.97</v>
       </c>
       <c r="O16" s="2">
         <v>185459.35</v>
@@ -1397,7 +1397,7 @@
         <v>5666</v>
       </c>
       <c r="Q16" s="2">
-        <v>81834.27</v>
+        <v>48651.38</v>
       </c>
       <c r="R16" s="1">
         <v>98.23999999999999</v>
@@ -1414,10 +1414,10 @@
         <v>10413</v>
       </c>
       <c r="D17" s="2">
-        <v>970394.76</v>
+        <v>966600.16</v>
       </c>
       <c r="E17" s="2">
-        <v>624019.96</v>
+        <v>619023.71</v>
       </c>
       <c r="F17" s="2">
         <v>346190.78</v>
@@ -1426,25 +1426,25 @@
         <v>28888.2</v>
       </c>
       <c r="H17" s="2">
-        <v>27724.78</v>
+        <v>27521.81</v>
       </c>
       <c r="I17" s="2">
-        <v>28202.46</v>
+        <v>27993.65</v>
       </c>
       <c r="J17" s="2">
-        <v>26689.13</v>
+        <v>26724.67</v>
       </c>
       <c r="K17" s="2">
-        <v>959981.76</v>
+        <v>956187.16</v>
       </c>
       <c r="L17" s="2">
-        <v>-21449.92</v>
+        <v>-25263.92</v>
       </c>
       <c r="M17" s="1">
-        <v>-2.06</v>
+        <v>-2.43</v>
       </c>
       <c r="N17" s="2">
-        <v>-21633.93</v>
+        <v>-26649.58</v>
       </c>
       <c r="O17" s="2">
         <v>0</v>
@@ -1453,7 +1453,7 @@
         <v>0</v>
       </c>
       <c r="Q17" s="2">
-        <v>-21633.93</v>
+        <v>-26649.58</v>
       </c>
       <c r="R17" s="1">
         <v>82.59999999999999</v>

</xml_diff>